<commit_message>
sutvarkyta iki 06 10 bendri
</commit_message>
<xml_diff>
--- a/Dienynas JAVA.xlsx
+++ b/Dienynas JAVA.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="146">
   <si>
     <t>mėnuo / diena</t>
   </si>
@@ -445,6 +445,21 @@
   </si>
   <si>
     <t>mirė Aliaus tėtis</t>
+  </si>
+  <si>
+    <t>06 06</t>
+  </si>
+  <si>
+    <t>06 07</t>
+  </si>
+  <si>
+    <t>06 10</t>
+  </si>
+  <si>
+    <t>pagrindai</t>
+  </si>
+  <si>
+    <t>atšakos (branch)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +546,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -644,31 +659,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
+      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -677,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -801,18 +796,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1120,7 +1103,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,7 +2617,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,7 +3393,7 @@
       </c>
       <c r="AF17" s="10"/>
     </row>
-    <row r="18" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -4686,7 +4669,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4778,10 +4761,18 @@
       <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -4822,10 +4813,18 @@
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="9">
+        <v>10</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -4860,10 +4859,18 @@
       <c r="B5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -4884,7 +4891,9 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="10"/>
+      <c r="AB5" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="AC5" s="10">
         <v>8</v>
       </c>
@@ -4906,7 +4915,9 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -4927,7 +4938,9 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="10"/>
+      <c r="AB6" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="AC6" s="10">
         <v>8</v>
       </c>
@@ -5161,7 +5174,9 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="10"/>
+      <c r="AB12" s="10" t="s">
+        <v>142</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -5200,7 +5215,9 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="10"/>
+      <c r="AB13" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="AC13" s="10">
         <v>8</v>
       </c>
@@ -7816,10 +7833,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F31"/>
+  <dimension ref="A2:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8122,7 +8139,7 @@
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="45" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="45"/>
@@ -8137,10 +8154,10 @@
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -8151,10 +8168,10 @@
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="48"/>
+      <c r="E23" s="46"/>
       <c r="F23" t="s">
         <v>134</v>
       </c>
@@ -8166,10 +8183,10 @@
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="50"/>
+      <c r="E24" s="45"/>
       <c r="F24" t="s">
         <v>139</v>
       </c>
@@ -8178,7 +8195,10 @@
       <c r="B25" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="45"/>
@@ -8190,7 +8210,10 @@
       <c r="B26" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E26" s="45"/>
@@ -8202,7 +8225,10 @@
       <c r="B27" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="45"/>
@@ -8214,20 +8240,37 @@
       <c r="B28" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="45" t="s">
         <v>40</v>
       </c>
       <c r="E28" s="45"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="45"/>
+    </row>
+    <row r="30" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>136</v>
       </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="45"/>
       <c r="F30" t="s">
         <v>140</v>
       </c>
@@ -8236,20 +8279,67 @@
       <c r="B31" t="s">
         <v>137</v>
       </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="45"/>
       <c r="F31" t="s">
         <v>138</v>
       </c>
     </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="45"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="45"/>
+      <c r="F33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="45"/>
+      <c r="F34" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
+  <mergeCells count="30">
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -8266,6 +8356,14 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sutvarkytas bendras žurnalas iki 07 26
</commit_message>
<xml_diff>
--- a/Dienynas JAVA.xlsx
+++ b/Dienynas JAVA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="12960" windowHeight="6300" tabRatio="793" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="12960" windowHeight="6300" tabRatio="793"/>
   </bookViews>
   <sheets>
     <sheet name="1. Tarnyb. stotys" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="188">
   <si>
     <t>mėnuo / diena</t>
   </si>
@@ -460,6 +460,132 @@
   </si>
   <si>
     <t>atšakos (branch)</t>
+  </si>
+  <si>
+    <t>06 11</t>
+  </si>
+  <si>
+    <t>06 12</t>
+  </si>
+  <si>
+    <t>06 13</t>
+  </si>
+  <si>
+    <t>06 14</t>
+  </si>
+  <si>
+    <t>06 17</t>
+  </si>
+  <si>
+    <t>06 18</t>
+  </si>
+  <si>
+    <t>06 19</t>
+  </si>
+  <si>
+    <t>06 20</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>06 21</t>
+  </si>
+  <si>
+    <t>06 26</t>
+  </si>
+  <si>
+    <t>06 27</t>
+  </si>
+  <si>
+    <t>06 28</t>
+  </si>
+  <si>
+    <t>06 29</t>
+  </si>
+  <si>
+    <t>06 30</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>07 01</t>
+  </si>
+  <si>
+    <t>07 02</t>
+  </si>
+  <si>
+    <t>07 03</t>
+  </si>
+  <si>
+    <t>07 04</t>
+  </si>
+  <si>
+    <t>07 05</t>
+  </si>
+  <si>
+    <t>07 08</t>
+  </si>
+  <si>
+    <t>07 09</t>
+  </si>
+  <si>
+    <t>07 10</t>
+  </si>
+  <si>
+    <t>07 11</t>
+  </si>
+  <si>
+    <t>07 12</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>07 15</t>
+  </si>
+  <si>
+    <t>07 16</t>
+  </si>
+  <si>
+    <t>07 17</t>
+  </si>
+  <si>
+    <t>07 18</t>
+  </si>
+  <si>
+    <t>07 19</t>
+  </si>
+  <si>
+    <t>07 22</t>
+  </si>
+  <si>
+    <t>07 23</t>
+  </si>
+  <si>
+    <t>07 24</t>
+  </si>
+  <si>
+    <t>07 25</t>
+  </si>
+  <si>
+    <t>07 26</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,11 +1321,21 @@
       <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -1239,11 +1375,21 @@
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41"/>
       <c r="B4" s="42"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -1301,7 +1447,9 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="18"/>
+      <c r="AB5" s="18" t="s">
+        <v>183</v>
+      </c>
       <c r="AC5" s="10">
         <v>8</v>
       </c>
@@ -1344,7 +1492,9 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="18"/>
+      <c r="AB6" s="18" t="s">
+        <v>184</v>
+      </c>
       <c r="AC6" s="10">
         <v>4</v>
       </c>
@@ -1383,7 +1533,9 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="18"/>
+      <c r="AB7" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="AC7" s="10">
         <v>4</v>
       </c>
@@ -1422,7 +1574,9 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="18"/>
+      <c r="AB8" s="18" t="s">
+        <v>186</v>
+      </c>
       <c r="AC8" s="10">
         <v>8</v>
       </c>
@@ -1461,7 +1615,9 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="18"/>
+      <c r="AB9" s="18" t="s">
+        <v>187</v>
+      </c>
       <c r="AC9" s="10">
         <v>8</v>
       </c>
@@ -3450,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4399,7 +4555,9 @@
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="10"/>
-      <c r="AB21" s="10"/>
+      <c r="AB21" s="10" t="s">
+        <v>178</v>
+      </c>
       <c r="AC21" s="10">
         <v>8</v>
       </c>
@@ -4439,7 +4597,9 @@
       <c r="Y22" s="10"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="10"/>
-      <c r="AB22" s="10"/>
+      <c r="AB22" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="AC22" s="10">
         <v>8</v>
       </c>
@@ -4479,7 +4639,9 @@
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="10"/>
-      <c r="AB23" s="10"/>
+      <c r="AB23" s="10" t="s">
+        <v>180</v>
+      </c>
       <c r="AC23" s="10">
         <v>8</v>
       </c>
@@ -4519,7 +4681,9 @@
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
-      <c r="AB24" s="10"/>
+      <c r="AB24" s="10" t="s">
+        <v>181</v>
+      </c>
       <c r="AC24" s="10">
         <v>8</v>
       </c>
@@ -4559,7 +4723,9 @@
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
       <c r="AA25" s="10"/>
-      <c r="AB25" s="10"/>
+      <c r="AB25" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="AC25" s="10">
         <v>8</v>
       </c>
@@ -4669,7 +4835,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4773,8 +4939,12 @@
       <c r="F3" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="G3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -4825,8 +4995,12 @@
       <c r="F4" s="9">
         <v>10</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="G4" s="9">
+        <v>11</v>
+      </c>
+      <c r="H4" s="9">
+        <v>12</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -4979,7 +5153,9 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="10"/>
+      <c r="AB7" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="AC7" s="10">
         <v>8</v>
       </c>
@@ -5256,7 +5432,9 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="10"/>
+      <c r="AB14" s="10" t="s">
+        <v>146</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>
@@ -5365,7 +5543,7 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5457,12 +5635,24 @@
       <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>96</v>
+      </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
@@ -5501,12 +5691,24 @@
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>158</v>
+      </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -5723,7 +5925,9 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="10"/>
+      <c r="AB9" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="AC9" s="10">
         <v>8</v>
       </c>
@@ -5762,7 +5966,9 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="10"/>
+      <c r="AB10" s="10" t="s">
+        <v>149</v>
+      </c>
       <c r="AC10" s="10">
         <v>8</v>
       </c>
@@ -5801,7 +6007,9 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="10"/>
+      <c r="AB11" s="10" t="s">
+        <v>150</v>
+      </c>
       <c r="AC11" s="10">
         <v>8</v>
       </c>
@@ -5840,7 +6048,9 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="10"/>
+      <c r="AB12" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -5879,7 +6089,9 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="10"/>
+      <c r="AB13" s="10" t="s">
+        <v>152</v>
+      </c>
       <c r="AC13" s="10">
         <v>8</v>
       </c>
@@ -5918,7 +6130,9 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="10"/>
+      <c r="AB14" s="10" t="s">
+        <v>153</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>
@@ -6065,8 +6279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE50" sqref="AE50"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6158,21 +6372,51 @@
       <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
@@ -6202,21 +6446,51 @@
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>177</v>
+      </c>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
@@ -6264,7 +6538,9 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="18"/>
+      <c r="AB5" s="18" t="s">
+        <v>160</v>
+      </c>
       <c r="AC5" s="10">
         <v>8</v>
       </c>
@@ -6307,7 +6583,9 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="18"/>
+      <c r="AB6" s="18" t="s">
+        <v>161</v>
+      </c>
       <c r="AC6" s="10">
         <v>8</v>
       </c>
@@ -6346,7 +6624,9 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="18"/>
+      <c r="AB7" s="18" t="s">
+        <v>162</v>
+      </c>
       <c r="AC7" s="10">
         <v>8</v>
       </c>
@@ -6424,7 +6704,9 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="18"/>
+      <c r="AB9" s="18" t="s">
+        <v>163</v>
+      </c>
       <c r="AC9" s="10">
         <v>8</v>
       </c>
@@ -6463,7 +6745,9 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="18"/>
+      <c r="AB10" s="18" t="s">
+        <v>164</v>
+      </c>
       <c r="AC10" s="10">
         <v>8</v>
       </c>
@@ -6502,7 +6786,9 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="18"/>
+      <c r="AB11" s="18" t="s">
+        <v>165</v>
+      </c>
       <c r="AC11" s="10">
         <v>8</v>
       </c>
@@ -6541,7 +6827,9 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="18"/>
+      <c r="AB12" s="18" t="s">
+        <v>167</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -6580,7 +6868,9 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="18"/>
+      <c r="AB13" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="AC13" s="10">
         <v>8</v>
       </c>
@@ -6619,7 +6909,9 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="18"/>
+      <c r="AB14" s="18" t="s">
+        <v>169</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>
@@ -6697,7 +6989,9 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
-      <c r="AB16" s="18"/>
+      <c r="AB16" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="AC16" s="10">
         <v>8</v>
       </c>
@@ -6736,7 +7030,9 @@
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
-      <c r="AB17" s="18"/>
+      <c r="AB17" s="18" t="s">
+        <v>171</v>
+      </c>
       <c r="AC17" s="10">
         <v>8</v>
       </c>
@@ -6775,7 +7071,9 @@
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
       <c r="Z18" s="10"/>
-      <c r="AB18" s="18"/>
+      <c r="AB18" s="18" t="s">
+        <v>172</v>
+      </c>
       <c r="AC18" s="10">
         <v>8</v>
       </c>
@@ -6814,7 +7112,9 @@
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
-      <c r="AB19" s="18"/>
+      <c r="AB19" s="18" t="s">
+        <v>173</v>
+      </c>
       <c r="AC19" s="10">
         <v>8</v>
       </c>
@@ -6853,7 +7153,9 @@
       <c r="X20" s="10"/>
       <c r="Y20" s="10"/>
       <c r="Z20" s="10"/>
-      <c r="AB20" s="18"/>
+      <c r="AB20" s="18" t="s">
+        <v>174</v>
+      </c>
       <c r="AC20" s="10">
         <v>8</v>
       </c>
@@ -6892,7 +7194,9 @@
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
-      <c r="AB21" s="18"/>
+      <c r="AB21" s="18" t="s">
+        <v>175</v>
+      </c>
       <c r="AC21" s="10">
         <v>8</v>
       </c>
@@ -7048,7 +7352,9 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
-      <c r="AB25" s="18"/>
+      <c r="AB25" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="AC25" s="10">
         <v>8</v>
       </c>
@@ -7835,8 +8141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8334,12 +8640,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -8356,14 +8664,12 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>